<commit_message>
Modified tests and added test cases in excel
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AD04C9-3BFB-1E42-9E67-AB9FC928E060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26880" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="F01.BVA" sheetId="3" r:id="rId3"/>
     <sheet name="BBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,12 +86,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="M19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -352,39 +351,12 @@
     <t>titlu</t>
   </si>
   <si>
-    <t>regizor</t>
-  </si>
-  <si>
-    <t>an aparitie</t>
-  </si>
-  <si>
-    <t>actori</t>
-  </si>
-  <si>
-    <t>categorie</t>
-  </si>
-  <si>
-    <t>cuvinte cheie</t>
-  </si>
-  <si>
     <t>expected</t>
   </si>
   <si>
-    <t>"Movie Title"</t>
-  </si>
-  <si>
-    <t>Actor1, Actor2</t>
-  </si>
-  <si>
-    <t>keyword1, keyword2</t>
-  </si>
-  <si>
     <t>2,3,2</t>
   </si>
   <si>
-    <t>record added</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -397,15 +369,6 @@
     <t>""</t>
   </si>
   <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t>201q</t>
-  </si>
-  <si>
-    <t>Error message-? Compiler checked</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -436,18 +399,6 @@
     <t>TC3_EC</t>
   </si>
   <si>
-    <t>"M"</t>
-  </si>
-  <si>
-    <t>Drama</t>
-  </si>
-  <si>
-    <t>"M…123"</t>
-  </si>
-  <si>
-    <t>"M…12"</t>
-  </si>
-  <si>
     <t>BBT TCs</t>
   </si>
   <si>
@@ -472,25 +423,13 @@
     <t>TC1_ECP</t>
   </si>
   <si>
-    <t>Director1, Director2</t>
-  </si>
-  <si>
     <t>TC3_ECP</t>
   </si>
   <si>
-    <t>Error message-Empty movie title</t>
-  </si>
-  <si>
-    <t>TC5_ECP</t>
-  </si>
-  <si>
     <t>TC3_BVA</t>
   </si>
   <si>
     <t>TC4_BVA</t>
-  </si>
-  <si>
-    <t>TC5_BVA</t>
   </si>
   <si>
     <t>Statistics</t>
@@ -952,12 +891,30 @@
   <si>
     <t>repeated task entry created</t>
   </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>TC2_ECP</t>
+  </si>
+  <si>
+    <t>TC4_ECP</t>
+  </si>
+  <si>
+    <t>4/3/2025 7:00:00PM</t>
+  </si>
+  <si>
+    <t>TC1_BVA</t>
+  </si>
+  <si>
+    <t>TC2_BVA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1039,26 +996,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -1069,14 +1008,6 @@
       <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1651,7 +1582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1661,28 +1592,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1709,7 +1633,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1719,11 +1642,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1733,25 +1656,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1773,7 +1696,41 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1788,6 +1745,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1818,11 +1783,47 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1830,49 +1831,32 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1884,38 +1868,26 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1926,18 +1898,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1959,10 +1919,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2010,57 +1970,59 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2099,7 +2061,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719ED11E-0B98-3B39-BE78-8971F85E5770}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719ED11E-0B98-3B39-BE78-8971F85E5770}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2129,9 +2091,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2169,9 +2131,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2206,7 +2168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2241,7 +2203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2414,46 +2376,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="9" max="9" width="32.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="32.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C1" s="54" t="s">
+    <row r="1" spans="2:10">
+      <c r="C1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56"/>
-      <c r="H1" s="45" t="s">
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="62"/>
+      <c r="H1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H2" s="57" t="s">
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="H2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+    </row>
+    <row r="3" spans="2:10">
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
         <v>3</v>
@@ -2462,74 +2424,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10">
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="J4" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10">
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="J5" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="31"/>
+    <row r="6" spans="2:10">
+      <c r="B6" s="25"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="J6" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+    <row r="7" spans="2:10" ht="14.5" customHeight="1"/>
+    <row r="8" spans="2:10">
+      <c r="B8" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -2537,7 +2499,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -2545,7 +2507,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2553,32 +2515,32 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="43" t="s">
+    <row r="18" spans="1:15">
+      <c r="B18" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C20" s="41" t="s">
+    <row r="20" spans="1:15">
+      <c r="C20" s="35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15">
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2595,7 +2557,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2612,222 +2574,221 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="53" t="s">
+    <row r="24" spans="1:15" ht="14.5" customHeight="1">
+      <c r="A24" s="36"/>
+      <c r="B24" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C26" s="44"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B31" s="133" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="134"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="134"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="134"/>
-      <c r="I31" s="134"/>
-      <c r="J31" s="134"/>
-      <c r="K31" s="134"/>
-      <c r="L31" s="134"/>
-      <c r="M31" s="134"/>
-      <c r="N31" s="134"/>
-      <c r="O31" s="134"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B32" s="134"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="134"/>
-      <c r="I32" s="134"/>
-      <c r="J32" s="134"/>
-      <c r="K32" s="134"/>
-      <c r="L32" s="134"/>
-      <c r="M32" s="134"/>
-      <c r="N32" s="134"/>
-      <c r="O32" s="134"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B33" s="134"/>
-      <c r="C33" s="134"/>
-      <c r="D33" s="134"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="134"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="134"/>
-      <c r="I33" s="134"/>
-      <c r="J33" s="134"/>
-      <c r="K33" s="134"/>
-      <c r="L33" s="134"/>
-      <c r="M33" s="134"/>
-      <c r="N33" s="134"/>
-      <c r="O33" s="134"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B58" s="132"/>
-      <c r="C58" s="132"/>
-      <c r="D58" s="132"/>
-      <c r="E58" s="132"/>
-      <c r="F58" s="132"/>
-      <c r="G58" s="132"/>
-      <c r="H58" s="132"/>
-      <c r="I58" s="132"/>
-      <c r="J58" s="132"/>
-      <c r="K58" s="132"/>
-      <c r="L58" s="132"/>
-      <c r="M58" s="132"/>
-      <c r="N58" s="132"/>
-      <c r="O58" s="132"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B59" s="132" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="132"/>
-      <c r="D59" s="132"/>
-      <c r="E59" s="132"/>
-      <c r="F59" s="132"/>
-      <c r="G59" s="132"/>
-      <c r="H59" s="132"/>
-      <c r="I59" s="132"/>
-      <c r="J59" s="132"/>
-      <c r="K59" s="132"/>
-      <c r="L59" s="132"/>
-      <c r="M59" s="132"/>
-      <c r="N59" s="132"/>
-      <c r="O59" s="132"/>
-    </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B60" s="132" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="132"/>
-      <c r="D60" s="132"/>
-      <c r="E60" s="132"/>
-      <c r="F60" s="132"/>
-      <c r="G60" s="132"/>
-      <c r="H60" s="132"/>
-      <c r="I60" s="132"/>
-      <c r="J60" s="132"/>
-      <c r="K60" s="132"/>
-      <c r="L60" s="132"/>
-      <c r="M60" s="132"/>
-      <c r="N60" s="132"/>
-      <c r="O60" s="132"/>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B61" s="132" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" s="132"/>
-      <c r="D61" s="132"/>
-      <c r="E61" s="132"/>
-      <c r="F61" s="132"/>
-      <c r="G61" s="132"/>
-      <c r="H61" s="132"/>
-      <c r="I61" s="132"/>
-      <c r="J61" s="132"/>
-      <c r="K61" s="132"/>
-      <c r="L61" s="132"/>
-      <c r="M61" s="132"/>
-      <c r="N61" s="132"/>
-      <c r="O61" s="132"/>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B62" s="135" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="135"/>
-      <c r="D62" s="135"/>
-      <c r="E62" s="135"/>
-      <c r="F62" s="135"/>
-      <c r="G62" s="135"/>
-      <c r="H62" s="135"/>
-      <c r="I62" s="135"/>
-      <c r="J62" s="135"/>
-      <c r="K62" s="135"/>
-      <c r="L62" s="135"/>
-      <c r="M62" s="135"/>
-      <c r="N62" s="135"/>
-      <c r="O62" s="135"/>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B63" s="135" t="s">
-        <v>101</v>
-      </c>
-      <c r="C63" s="135"/>
-      <c r="D63" s="135"/>
-      <c r="E63" s="135"/>
-      <c r="F63" s="135"/>
-      <c r="G63" s="135"/>
-      <c r="H63" s="135"/>
-      <c r="I63" s="135"/>
-      <c r="J63" s="135"/>
-      <c r="K63" s="135"/>
-      <c r="L63" s="135"/>
-      <c r="M63" s="135"/>
-      <c r="N63" s="135"/>
-      <c r="O63" s="135"/>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B64" s="135" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="135"/>
-      <c r="D64" s="135"/>
-      <c r="E64" s="135"/>
-      <c r="F64" s="135"/>
-      <c r="G64" s="135"/>
-      <c r="H64" s="135"/>
-      <c r="I64" s="135"/>
-      <c r="J64" s="135"/>
-      <c r="K64" s="135"/>
-      <c r="L64" s="135"/>
-      <c r="M64" s="135"/>
-      <c r="N64" s="135"/>
-      <c r="O64" s="135"/>
-    </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B65" s="132" t="s">
-        <v>103</v>
-      </c>
-      <c r="C65" s="132"/>
-      <c r="D65" s="132"/>
-      <c r="E65" s="132"/>
-      <c r="F65" s="132"/>
-      <c r="G65" s="132"/>
-      <c r="H65" s="132"/>
-      <c r="I65" s="132"/>
-      <c r="J65" s="132"/>
-      <c r="K65" s="132"/>
-      <c r="L65" s="132"/>
-      <c r="M65" s="132"/>
-      <c r="N65" s="132"/>
-      <c r="O65" s="132"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="C26" s="38"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="B31" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="65"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="65"/>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="66"/>
+      <c r="L58" s="66"/>
+      <c r="M58" s="66"/>
+      <c r="N58" s="66"/>
+      <c r="O58" s="66"/>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="B59" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="66"/>
+      <c r="D59" s="66"/>
+      <c r="E59" s="66"/>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="66"/>
+      <c r="L59" s="66"/>
+      <c r="M59" s="66"/>
+      <c r="N59" s="66"/>
+      <c r="O59" s="66"/>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="B60" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="66"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="66"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="66"/>
+      <c r="L60" s="66"/>
+      <c r="M60" s="66"/>
+      <c r="N60" s="66"/>
+      <c r="O60" s="66"/>
+    </row>
+    <row r="61" spans="2:15">
+      <c r="B61" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="L61" s="66"/>
+      <c r="M61" s="66"/>
+      <c r="N61" s="66"/>
+      <c r="O61" s="66"/>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="B62" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="67"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="67"/>
+      <c r="F62" s="67"/>
+      <c r="G62" s="67"/>
+      <c r="H62" s="67"/>
+      <c r="I62" s="67"/>
+      <c r="J62" s="67"/>
+      <c r="K62" s="67"/>
+      <c r="L62" s="67"/>
+      <c r="M62" s="67"/>
+      <c r="N62" s="67"/>
+      <c r="O62" s="67"/>
+    </row>
+    <row r="63" spans="2:15">
+      <c r="B63" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="67"/>
+      <c r="F63" s="67"/>
+      <c r="G63" s="67"/>
+      <c r="H63" s="67"/>
+      <c r="I63" s="67"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="67"/>
+      <c r="L63" s="67"/>
+      <c r="M63" s="67"/>
+      <c r="N63" s="67"/>
+      <c r="O63" s="67"/>
+    </row>
+    <row r="64" spans="2:15">
+      <c r="B64" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="67"/>
+      <c r="G64" s="67"/>
+      <c r="H64" s="67"/>
+      <c r="I64" s="67"/>
+      <c r="J64" s="67"/>
+      <c r="K64" s="67"/>
+      <c r="L64" s="67"/>
+      <c r="M64" s="67"/>
+      <c r="N64" s="67"/>
+      <c r="O64" s="67"/>
+    </row>
+    <row r="65" spans="2:15">
+      <c r="B65" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="66"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="66"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="66"/>
+      <c r="H65" s="66"/>
+      <c r="I65" s="66"/>
+      <c r="J65" s="66"/>
+      <c r="K65" s="66"/>
+      <c r="L65" s="66"/>
+      <c r="M65" s="66"/>
+      <c r="N65" s="66"/>
+      <c r="O65" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B58:O58"/>
     <mergeCell ref="B65:O65"/>
     <mergeCell ref="B59:O59"/>
     <mergeCell ref="B60:O60"/>
@@ -2839,6 +2800,7 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="B31:O33"/>
+    <mergeCell ref="B58:O58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2847,518 +2809,518 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12:Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" customWidth="1"/>
-    <col min="16" max="16" width="40.5" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1"/>
+    <col min="16" max="16" width="40.453125" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="2:17">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="56"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="63"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="64" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="G5" s="65" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="G5" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="19" t="s">
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="66" t="s">
+      <c r="G6" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="78" t="s">
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="78"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="Q6" s="90"/>
+    </row>
+    <row r="7" spans="2:17">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="58" t="s">
-        <v>104</v>
+      <c r="C7" s="68" t="s">
+        <v>84</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="N7" s="74" t="s">
-        <v>116</v>
-      </c>
-      <c r="O7" s="75"/>
-      <c r="P7" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q7" s="75"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="G7" s="77"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="N7" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="O7" s="87"/>
+      <c r="P7" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="87"/>
+    </row>
+    <row r="8" spans="2:17">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="4" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="148"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="27"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G8" s="46"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="21"/>
+    </row>
+    <row r="9" spans="2:17">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="19">
+        <v>86</v>
+      </c>
+      <c r="G9" s="14">
         <v>1</v>
       </c>
       <c r="H9" s="2">
         <v>2</v>
       </c>
-      <c r="I9" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" s="137">
+      <c r="I9" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="48">
         <v>45750.666666666664</v>
       </c>
-      <c r="K9" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="L9" s="46" t="b">
+      <c r="K9" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="M9" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="N9" s="72" t="b">
+      <c r="M9" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="84" t="b">
         <v>1</v>
       </c>
-      <c r="O9" s="73" t="s">
-        <v>42</v>
-      </c>
-      <c r="P9" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q9" s="73"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="O9" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q9" s="85"/>
+    </row>
+    <row r="10" spans="2:17">
       <c r="B10" s="4"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="G10" s="19">
+      <c r="G10" s="14">
         <v>2</v>
       </c>
       <c r="H10" s="2">
         <v>4</v>
       </c>
-      <c r="I10" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="J10" s="137">
+      <c r="I10" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="48">
         <v>45752</v>
       </c>
-      <c r="K10" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="L10" s="46" t="b">
+      <c r="K10" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="M10" s="46">
+      <c r="M10" s="40">
         <v>0</v>
       </c>
-      <c r="N10" s="72" t="b">
+      <c r="N10" s="84" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="147"/>
-      <c r="P10" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q10" s="48"/>
-    </row>
-    <row r="11" spans="2:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O10" s="96"/>
+      <c r="P10" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q10" s="42"/>
+    </row>
+    <row r="11" spans="2:17" ht="45" customHeight="1">
       <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C11" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="136" t="s">
-        <v>109</v>
+      <c r="C11" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>89</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="G11" s="16">
+      <c r="G11" s="11">
         <v>3</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="10">
         <v>1</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="J11" s="144">
+      <c r="I11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="51">
         <v>45750.666666666664</v>
       </c>
-      <c r="K11" s="144">
+      <c r="K11" s="51">
         <v>45751.666666666664</v>
       </c>
-      <c r="L11" s="17" t="b">
+      <c r="L11" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="12">
         <v>3600</v>
       </c>
-      <c r="N11" s="145" t="b">
+      <c r="N11" s="80" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="146" t="s">
-        <v>46</v>
-      </c>
-      <c r="P11" s="145" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q11" s="146"/>
-    </row>
-    <row r="12" spans="2:17" ht="48" x14ac:dyDescent="0.2">
+      <c r="O11" s="81" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q11" s="81"/>
+    </row>
+    <row r="12" spans="2:17" ht="43.5">
       <c r="B12" s="4">
         <v>5</v>
       </c>
-      <c r="C12" s="81"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="136" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" s="16">
+      <c r="E12" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="11">
         <v>4</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="10">
         <v>5</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="J12" s="144">
+      <c r="I12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="51">
         <v>45748.4375</v>
       </c>
-      <c r="K12" s="144">
+      <c r="K12" s="51">
         <v>45748.375</v>
       </c>
-      <c r="L12" s="17" t="b">
+      <c r="L12" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="12">
         <v>1800</v>
       </c>
-      <c r="N12" s="145" t="b">
+      <c r="N12" s="80" t="b">
         <v>0</v>
       </c>
-      <c r="O12" s="146"/>
-      <c r="P12" s="145" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q12" s="146"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="O12" s="81"/>
+      <c r="P12" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q12" s="81"/>
+    </row>
+    <row r="13" spans="2:17">
       <c r="B13" s="4">
         <v>6</v>
       </c>
-      <c r="C13" s="59" t="s">
-        <v>44</v>
+      <c r="C13" s="69" t="s">
+        <v>35</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="G13" s="19">
+      <c r="G13" s="14">
         <v>5</v>
       </c>
-      <c r="H13" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="K13" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="L13" s="138" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="N13" s="139" t="s">
-        <v>44</v>
-      </c>
-      <c r="O13" s="140"/>
-      <c r="P13" s="139" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q13" s="140"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H13" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="83"/>
+      <c r="P13" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" s="83"/>
+    </row>
+    <row r="14" spans="2:17">
       <c r="B14" s="4">
         <v>7</v>
       </c>
-      <c r="C14" s="60"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="G14" s="19">
+      <c r="G14" s="14">
         <v>6</v>
       </c>
-      <c r="H14" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="L14" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="M14" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="N14" s="141" t="s">
-        <v>44</v>
-      </c>
-      <c r="O14" s="142"/>
-      <c r="P14" s="139" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q14" s="140"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H14" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="79"/>
+      <c r="P14" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="83"/>
+    </row>
+    <row r="15" spans="2:17">
       <c r="B15" s="4">
         <v>8</v>
       </c>
-      <c r="C15" s="58" t="s">
-        <v>44</v>
+      <c r="C15" s="68" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="G15" s="19">
+      <c r="G15" s="14">
         <v>7</v>
       </c>
-      <c r="H15" s="138" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="138"/>
-      <c r="J15" s="138"/>
-      <c r="K15" s="138"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="138"/>
-      <c r="N15" s="139"/>
-      <c r="O15" s="140"/>
-      <c r="P15" s="139"/>
-      <c r="Q15" s="140"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H15" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="83"/>
+    </row>
+    <row r="16" spans="2:17">
       <c r="B16" s="4">
         <v>9</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="71"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G16" s="11"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="84"/>
+      <c r="O16" s="85"/>
+      <c r="P16" s="92"/>
+      <c r="Q16" s="93"/>
+    </row>
+    <row r="17" spans="2:17">
       <c r="B17" s="4">
         <v>10</v>
       </c>
-      <c r="C17" s="58" t="s">
-        <v>44</v>
+      <c r="C17" s="68" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="71"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G17" s="11"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="93"/>
+    </row>
+    <row r="18" spans="2:17">
       <c r="B18" s="4">
         <v>11</v>
       </c>
-      <c r="C18" s="58"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="71"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G18" s="11"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="84"/>
+      <c r="O18" s="85"/>
+      <c r="P18" s="92"/>
+      <c r="Q18" s="93"/>
+    </row>
+    <row r="19" spans="2:17">
       <c r="B19" s="4">
         <v>12</v>
       </c>
-      <c r="C19" s="58" t="s">
-        <v>44</v>
+      <c r="C19" s="68" t="s">
+        <v>35</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="G19" s="19"/>
+      <c r="G19" s="14"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="72"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="71"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N19" s="84"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="93"/>
+    </row>
+    <row r="20" spans="2:17">
       <c r="B20" s="4">
         <v>13</v>
       </c>
-      <c r="C20" s="58"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17">
       <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
+        <v>39</v>
+      </c>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -3369,26 +3331,22 @@
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P16:Q16"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="P19:Q19"/>
     <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P16:Q16"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N12:O12"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C9"/>
@@ -3401,566 +3359,567 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="N14:O14"/>
     <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="N7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:R25"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="F7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.5" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" customWidth="1"/>
-    <col min="18" max="18" width="9.5" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.36328125" customWidth="1"/>
+    <col min="16" max="16" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.36328125" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="2:18">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="56"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="149" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="63"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="87" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="104" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-    </row>
-    <row r="6" spans="2:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+    </row>
+    <row r="6" spans="2:18" ht="14.5" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="G6" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="76" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="G6" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="88" t="s">
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="89"/>
-    </row>
-    <row r="7" spans="2:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="59">
+      <c r="R6" s="106"/>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="69">
         <v>1</v>
       </c>
-      <c r="C7" s="82" t="s">
-        <v>124</v>
+      <c r="C7" s="94" t="s">
+        <v>104</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q7" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="R7" s="87"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="95"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" s="53">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="M8" s="53">
+        <v>45750.791666666664</v>
+      </c>
+      <c r="N8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8">
+        <v>1800</v>
+      </c>
+      <c r="P8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="107" t="s">
+        <v>118</v>
+      </c>
+      <c r="R8" s="108"/>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="95"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="11">
+        <v>2</v>
+      </c>
+      <c r="H9" s="12">
+        <v>2</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="L9" s="50">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9" s="110"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="95"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="14">
+        <v>3</v>
+      </c>
+      <c r="H10" s="9">
+        <v>7</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="53">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="M10" s="53">
+        <v>45750.417361111111</v>
+      </c>
+      <c r="N10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="8">
+        <v>60</v>
+      </c>
+      <c r="P10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="107" t="s">
+        <v>120</v>
+      </c>
+      <c r="R10" s="108"/>
+    </row>
+    <row r="11" spans="2:18" ht="43.5">
+      <c r="B11" s="69">
+        <v>2</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="G11" s="11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <v>5</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="50">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="M11" s="50">
+        <v>45750.415972222225</v>
+      </c>
+      <c r="N11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="13">
+        <v>60</v>
+      </c>
+      <c r="P11" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="R11" s="110"/>
+    </row>
+    <row r="12" spans="2:18" ht="43.5">
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="G12" s="14">
+        <v>5</v>
+      </c>
+      <c r="H12" s="9">
+        <v>7</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="108"/>
+    </row>
+    <row r="13" spans="2:18" ht="43.5">
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="N7" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q7" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="R7" s="75"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="81"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="19">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>2</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="L8" s="151">
-        <v>45750.416666666664</v>
-      </c>
-      <c r="M8" s="151">
-        <v>45750.791666666664</v>
-      </c>
-      <c r="N8" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8" s="13">
-        <v>1800</v>
-      </c>
-      <c r="P8" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="90" t="s">
-        <v>138</v>
-      </c>
-      <c r="R8" s="91"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="81"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="16">
-        <v>2</v>
-      </c>
-      <c r="H9" s="17">
-        <v>2</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="L9" s="143">
-        <v>45750.416666666664</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="N9" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="18">
-        <v>0</v>
-      </c>
-      <c r="P9" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="68" t="s">
-        <v>119</v>
-      </c>
-      <c r="R9" s="69"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="81"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="19">
+      <c r="G13" s="14">
+        <v>6</v>
+      </c>
+      <c r="H13" s="9">
+        <v>8</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="108"/>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="B14" s="69">
         <v>3</v>
       </c>
-      <c r="H10" s="14">
+      <c r="C14" s="94"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="14">
         <v>7</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="L10" s="151">
-        <v>45750.416666666664</v>
-      </c>
-      <c r="M10" s="151">
-        <v>45750.417361111111</v>
-      </c>
-      <c r="N10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O10" s="13">
-        <v>60</v>
-      </c>
-      <c r="P10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="90" t="s">
-        <v>140</v>
-      </c>
-      <c r="R10" s="91"/>
-    </row>
-    <row r="11" spans="2:18" ht="48" x14ac:dyDescent="0.2">
-      <c r="B11" s="59">
-        <v>2</v>
-      </c>
-      <c r="C11" s="82" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="150" t="s">
-        <v>131</v>
-      </c>
-      <c r="G11" s="16">
+      <c r="H14" s="9"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="108"/>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="B15" s="95"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="14">
+        <v>8</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="108"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="95"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="14">
+        <v>9</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="108"/>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="95"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="14">
+        <v>10</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="108"/>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="95"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="14">
+        <v>11</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="107"/>
+      <c r="R18" s="108"/>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="70"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="14">
+        <v>12</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="108"/>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="69">
         <v>4</v>
       </c>
-      <c r="H11" s="17">
-        <v>5</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="L11" s="143">
-        <v>45750.416666666664</v>
-      </c>
-      <c r="M11" s="143">
-        <v>45750.415972222225</v>
-      </c>
-      <c r="N11" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" s="18">
-        <v>60</v>
-      </c>
-      <c r="P11" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="68" t="s">
-        <v>119</v>
-      </c>
-      <c r="R11" s="69"/>
-    </row>
-    <row r="12" spans="2:18" ht="48" x14ac:dyDescent="0.2">
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="150" t="s">
-        <v>132</v>
-      </c>
-      <c r="G12" s="19">
-        <v>5</v>
-      </c>
-      <c r="H12" s="14">
-        <v>7</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="91"/>
-    </row>
-    <row r="13" spans="2:18" ht="48" x14ac:dyDescent="0.2">
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="150" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" s="19">
-        <v>6</v>
-      </c>
-      <c r="H13" s="14">
-        <v>8</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="91"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="59">
-        <v>3</v>
-      </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="19">
-        <v>7</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="91"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="81"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="19">
-        <v>8</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="91"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="81"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="19">
-        <v>9</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="90"/>
-      <c r="R16" s="91"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="81"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="19">
-        <v>10</v>
-      </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="90"/>
-      <c r="R17" s="91"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="81"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="19">
-        <v>11</v>
-      </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="91"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="60"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="19">
-        <v>12</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="90"/>
-      <c r="R19" s="91"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="59">
-        <v>4</v>
-      </c>
-      <c r="C20" s="82" t="s">
-        <v>44</v>
+      <c r="C20" s="94" t="s">
+        <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="19">
+        <v>35</v>
+      </c>
+      <c r="G20" s="14">
         <v>13</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="91"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="81"/>
-      <c r="C21" s="83"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="108"/>
+    </row>
+    <row r="21" spans="2:18">
+      <c r="B21" s="95"/>
+      <c r="C21" s="99"/>
       <c r="D21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="81"/>
-      <c r="C22" s="83"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18">
+      <c r="B22" s="95"/>
+      <c r="C22" s="99"/>
       <c r="D22" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="81"/>
-      <c r="C23" s="83"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="B23" s="95"/>
+      <c r="C23" s="99"/>
       <c r="D23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="37"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="81"/>
-      <c r="C24" s="83"/>
+        <v>35</v>
+      </c>
+      <c r="G23" s="98"/>
+      <c r="H23" s="98"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="103"/>
+      <c r="K23" s="103"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="31"/>
+    </row>
+    <row r="24" spans="2:18">
+      <c r="B24" s="95"/>
+      <c r="C24" s="99"/>
       <c r="D24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="85"/>
-      <c r="J24" s="85"/>
-      <c r="K24" s="85"/>
-      <c r="L24" s="85"/>
-      <c r="M24" s="85"/>
-      <c r="N24" s="38"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="60"/>
-      <c r="C25" s="84"/>
+        <v>35</v>
+      </c>
+      <c r="I24" s="101"/>
+      <c r="J24" s="101"/>
+      <c r="K24" s="101"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="101"/>
+      <c r="N24" s="32"/>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="70"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q16:R16"/>
     <mergeCell ref="Q11:R11"/>
     <mergeCell ref="K6:P6"/>
     <mergeCell ref="Q10:R10"/>
@@ -3977,6 +3936,9 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="Q8:R8"/>
     <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q16:R16"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
@@ -4001,620 +3963,646 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:P21"/>
+  <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.83203125" customWidth="1"/>
-    <col min="13" max="13" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" customWidth="1"/>
+    <col min="13" max="13" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="2:14">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="56"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="108" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="102" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="113" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="74" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="B3" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="115" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="78" t="s">
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="78"/>
-    </row>
-    <row r="5" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="112"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="22" t="s">
+      <c r="N4" s="90"/>
+    </row>
+    <row r="5" spans="2:14" ht="15" thickBot="1">
+      <c r="B5" s="121"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="112" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="113"/>
+      <c r="M5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="N5" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15" thickTop="1">
+      <c r="B6" s="15">
+        <v>1</v>
+      </c>
+      <c r="C6" s="119" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="142" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="148" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="149">
+        <v>45750.666666666664</v>
+      </c>
+      <c r="H6" s="148" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="148" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="148" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="150" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="151" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="M6" s="148" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="96"/>
-      <c r="M5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20">
-        <v>1</v>
-      </c>
-      <c r="C6" s="110" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="25">
-        <v>2010</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="97" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="11">
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="7">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="8">
-        <v>2010</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K7" s="104" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="105"/>
-      <c r="M7" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="11">
-        <f t="shared" ref="B8:B13" si="0">B7+1</f>
+      <c r="C7" s="119"/>
+      <c r="D7" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="143" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="147" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="152">
+        <v>45752</v>
+      </c>
+      <c r="H7" s="147" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="147">
+        <v>0</v>
+      </c>
+      <c r="K7" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="83"/>
+      <c r="M7" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="7">
+        <f t="shared" ref="B8:B12" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="110"/>
-      <c r="D8" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="11">
-        <f t="shared" si="0"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="143" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="144">
+        <v>45750.666666666664</v>
+      </c>
+      <c r="H8" s="144">
+        <v>45751.666666666664</v>
+      </c>
+      <c r="I8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>3600</v>
+      </c>
+      <c r="K8" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="108"/>
+      <c r="M8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="7"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="144">
+        <v>45748.4375</v>
+      </c>
+      <c r="H9" s="144">
+        <v>45748.375</v>
+      </c>
+      <c r="I9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1800</v>
+      </c>
+      <c r="K9" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="108"/>
+      <c r="M9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="7">
+        <f>B8+1</f>
         <v>4</v>
       </c>
-      <c r="C9" s="110"/>
-      <c r="D9" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="106" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="107"/>
-      <c r="M9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="11">
-        <f t="shared" si="0"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="145" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="146"/>
+      <c r="M10" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="7">
+        <f>B10+1</f>
         <v>5</v>
       </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="10">
-        <v>2010</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K10" s="99" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="100"/>
-      <c r="M10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="11">
+      <c r="C11" s="119"/>
+      <c r="D11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" s="144">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1800</v>
+      </c>
+      <c r="K11" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="108"/>
+      <c r="M11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N11" s="141" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="C12" s="119"/>
+      <c r="D12" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="53">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="108"/>
+      <c r="M12" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="141" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15" thickBot="1">
+      <c r="B13" s="157"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="153" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="154">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="H13" s="154">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="I13" s="153" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="153">
+        <v>60</v>
+      </c>
+      <c r="K13" s="155" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="156"/>
+      <c r="M13" s="153" t="s">
+        <v>120</v>
+      </c>
+      <c r="N13" s="158"/>
+    </row>
+    <row r="14" spans="2:14" ht="15.5" thickTop="1" thickBot="1">
+      <c r="B14" s="16" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C14" s="120"/>
+      <c r="D14" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="153" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="154">
+        <v>45750.416666666664</v>
+      </c>
+      <c r="H14" s="154">
+        <v>45750.415972222225</v>
+      </c>
+      <c r="I14" s="153" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="153">
+        <v>60</v>
+      </c>
+      <c r="K14" s="155" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="156"/>
+      <c r="M14" s="153" t="s">
+        <v>99</v>
+      </c>
+      <c r="N14" s="153" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15" thickTop="1">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="2:14" ht="14.5" customHeight="1">
+      <c r="B16" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="2:16" ht="15" thickBot="1">
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="2:16" ht="15" thickTop="1">
+      <c r="C18" s="130" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="130" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="10">
-        <v>2010</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="99" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" s="100"/>
-      <c r="M11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="110"/>
-      <c r="D12" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="I18" s="133"/>
+      <c r="J18" s="131"/>
+      <c r="K18" s="131"/>
+      <c r="L18" s="132"/>
+      <c r="M18" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="10">
-        <v>2010</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="99" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="100"/>
-      <c r="M12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21">
-        <f t="shared" si="0"/>
+      <c r="N18" s="133"/>
+      <c r="O18" s="131"/>
+      <c r="P18" s="132"/>
+    </row>
+    <row r="19" spans="2:16" ht="14.5" customHeight="1">
+      <c r="B19" s="126" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="127" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="128" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="129" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="138" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="134" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="135"/>
+      <c r="J19" s="128" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="129" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="139" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" s="128" t="s">
+        <v>65</v>
+      </c>
+      <c r="O19" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" s="129" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="126"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="128"/>
+      <c r="L20" s="129"/>
+      <c r="M20" s="140"/>
+      <c r="N20" s="128"/>
+      <c r="O20" s="128"/>
+      <c r="P20" s="129"/>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="26">
         <v>8</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="K13" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="L13" s="94"/>
-      <c r="M13" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="N13" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-    </row>
-    <row r="15" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="121" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="122"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="121" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="124"/>
-      <c r="J17" s="122"/>
-      <c r="K17" s="122"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="121" t="s">
-        <v>84</v>
-      </c>
-      <c r="N17" s="124"/>
-      <c r="O17" s="122"/>
-      <c r="P17" s="123"/>
-    </row>
-    <row r="18" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="117" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="119" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="119" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="120" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="129" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="125" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" s="126"/>
-      <c r="J18" s="119" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" s="119" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" s="120" t="s">
-        <v>87</v>
-      </c>
-      <c r="M18" s="130" t="s">
-        <v>90</v>
-      </c>
-      <c r="N18" s="119" t="s">
-        <v>85</v>
-      </c>
-      <c r="O18" s="119" t="s">
-        <v>86</v>
-      </c>
-      <c r="P18" s="120" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="117"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="129"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="119"/>
-      <c r="K19" s="119"/>
-      <c r="L19" s="120"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="119"/>
-      <c r="O19" s="119"/>
-      <c r="P19" s="120"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="36" t="s">
+      <c r="D21" s="28">
+        <v>5</v>
+      </c>
+      <c r="E21" s="28">
+        <v>3</v>
+      </c>
+      <c r="F21" s="29"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="124" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="32">
-        <v>8</v>
-      </c>
-      <c r="D20" s="34">
+      <c r="I21" s="125"/>
+      <c r="J21" s="2">
+        <v>3</v>
+      </c>
+      <c r="K21" s="28">
+        <v>3</v>
+      </c>
+      <c r="L21" s="29">
+        <v>0</v>
+      </c>
+      <c r="M21" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="N21" s="2">
         <v>5</v>
       </c>
-      <c r="E20" s="34">
-        <v>3</v>
-      </c>
-      <c r="F20" s="35"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="115" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="116"/>
-      <c r="J20" s="2">
-        <v>3</v>
-      </c>
-      <c r="K20" s="34">
-        <v>3</v>
-      </c>
-      <c r="L20" s="35">
+      <c r="O21" s="28">
+        <v>5</v>
+      </c>
+      <c r="P21" s="29">
         <v>0</v>
       </c>
-      <c r="M20" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="N20" s="2">
-        <v>5</v>
-      </c>
-      <c r="O20" s="34">
-        <v>5</v>
-      </c>
-      <c r="P20" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="M22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C6:C13"/>
+  <mergeCells count="38">
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C6:C14"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="K19:K20"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
     <mergeCell ref="F4:L4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K10:L10"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
     <mergeCell ref="B3:N3"/>
+    <mergeCell ref="K8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated lab2 docs. refactored parameterized tests for Jenkins compatibility.
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6968FA9-F00A-8040-ABE8-A910CB3D0D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26880" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -12,7 +13,7 @@
     <sheet name="F01.BVA" sheetId="3" r:id="rId3"/>
     <sheet name="BBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,12 +87,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H18" authorId="0" shapeId="0">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M18" authorId="0" shapeId="0">
+    <comment ref="M18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -145,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="119">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -183,141 +184,6 @@
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
   <si>
-    <t>1. Evidenţa filmelor din colecţia personală</t>
-  </si>
-  <si>
-    <t>Un cinefil doreşte să îşi dezvolte un program pentru gestionarea filmelor din colecţia personală. Programul va permite următoarele operaţii:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>F01.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> adăugarea unui film nou (titlu, regizor, an aparitie, actori, categorie, cuvinte cheie);</t>
-    </r>
-  </si>
-  <si>
-    <t>Observații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
-  </si>
-  <si>
-    <t>addMovie(String title, String director, int year, List&lt;String&gt; actors, String category, List&lt;String&gt; keywords): void</t>
-  </si>
-  <si>
-    <t>2. Metoda este definită la nivelul repository, service sau ui.</t>
-  </si>
-  <si>
-    <t>3. Se aleg doi parametri ai metodei testate şi se definesc condiţii asupra acestora. Condiţiile (constrângerile) rezultă din specificaţii.</t>
-  </si>
-  <si>
-    <t>4. Pentru aceşti parametri se aplică ECP şi BVA. La proiectarea testelor se consideră că parametrii de intrare neinvestigaţi aici au valori valide, adică folosim dummy objects.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Exemplu: Parametrii </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>title</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> şi </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>year</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">; Condiţii pentru aceşti parametri de intrare: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>title</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> este un string cu lungimea validă de la 1 la 255 caractere; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>year</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> este valid dacă ia valori între 1899 şi 2025.</t>
-    </r>
-  </si>
-  <si>
     <t>EC Identification</t>
   </si>
   <si>
@@ -394,9 +260,6 @@
   </si>
   <si>
     <t>expected result</t>
-  </si>
-  <si>
-    <t>TC3_EC</t>
   </si>
   <si>
     <t>BBT TCs</t>
@@ -760,9 +623,6 @@
     </r>
   </si>
   <si>
-    <t>title is String with length between 1 and 255</t>
-  </si>
-  <si>
     <t>len(title) = 0</t>
   </si>
   <si>
@@ -770,10 +630,6 @@
   </si>
   <si>
     <t>1 &lt;= len(title) &lt;= 255</t>
-  </si>
-  <si>
-    <t>endDateTime is a date after startDateTime if task is repeated, 
-otherwise it will be overwtitten to startDateTime value</t>
   </si>
   <si>
     <t>isRepeated = false
@@ -821,9 +677,6 @@
   </si>
   <si>
     <t>"Shopping"</t>
-  </si>
-  <si>
-    <t>title is String, length in [1,255]</t>
   </si>
   <si>
     <r>
@@ -852,78 +705,85 @@
     <t>04. titlu = "A".repeat(256), length = 256</t>
   </si>
   <si>
-    <t>endDateTime is a date after startDateTime 
+    <t>yes</t>
+  </si>
+  <si>
+    <t>"A"</t>
+  </si>
+  <si>
+    <t>task entry created with title "Meeting"</t>
+  </si>
+  <si>
+    <t>task entry created, with endDateTime = startEndTime</t>
+  </si>
+  <si>
+    <t>task entry created with title "A"</t>
+  </si>
+  <si>
+    <t>"A".repeat(256)</t>
+  </si>
+  <si>
+    <t>repeated task entry created</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>TC2_ECP</t>
+  </si>
+  <si>
+    <t>TC4_ECP</t>
+  </si>
+  <si>
+    <t>TC1_BVA</t>
+  </si>
+  <si>
+    <t>TC2_BVA</t>
+  </si>
+  <si>
+    <t>no bugs</t>
+  </si>
+  <si>
+    <t>Start time must be before end time</t>
+  </si>
+  <si>
+    <t>Title must be a non-empty string with a maximum length of 255 characters</t>
+  </si>
+  <si>
+    <t>title has length between 1 and 255</t>
+  </si>
+  <si>
+    <t>endDateTime is after startDateTime if task is repeated, 
+otherwise it will be overwtitten to startDateTime value</t>
+  </si>
+  <si>
+    <t>2, 4</t>
+  </si>
+  <si>
+    <t>title has length in (0,256)</t>
+  </si>
+  <si>
+    <t>endDateTime is after startDateTime 
 for a repeated task</t>
   </si>
   <si>
     <t>05. 
-endDateTime = 2025-04-03 09:59,
-startDateTime = 2025-04-03 10:00</t>
+endDateTime = startDateTime - 1</t>
   </si>
   <si>
     <t>06. 
-endDateTime = 2025-04-03 10:00,
-startDateTime = 2025-04-03 10:00</t>
+endDateTime = startDateTime</t>
   </si>
   <si>
     <t>07. 
-endDateTime = 2025-04-03 10:01,
-startDateTime = 2025-04-03 10:00</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>"A"</t>
-  </si>
-  <si>
-    <t>task entry created with title "Meeting"</t>
-  </si>
-  <si>
-    <t>task entry created, with endDateTime = startEndTime</t>
-  </si>
-  <si>
-    <t>task entry created with title "A"</t>
-  </si>
-  <si>
-    <t>"A".repeat(256)</t>
-  </si>
-  <si>
-    <t>repeated task entry created</t>
-  </si>
-  <si>
-    <t>Interval</t>
-  </si>
-  <si>
-    <t>TC2_ECP</t>
-  </si>
-  <si>
-    <t>TC4_ECP</t>
-  </si>
-  <si>
-    <t>4/3/2025 7:00:00PM</t>
-  </si>
-  <si>
-    <t>TC1_BVA</t>
-  </si>
-  <si>
-    <t>TC2_BVA</t>
-  </si>
-  <si>
-    <t>no bugs</t>
-  </si>
-  <si>
-    <t>Start time must be before end time</t>
-  </si>
-  <si>
-    <t>Title must be a non-empty string with a maximum length of 255 characters</t>
+endDateTime = startDateTime + 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -962,21 +822,6 @@
       <b/>
       <sz val="11"/>
       <color indexed="17"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="30"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color indexed="30"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1591,9 +1436,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1601,63 +1446,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1665,25 +1510,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1693,16 +1538,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1711,57 +1556,79 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1780,35 +1647,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1816,28 +1677,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1846,11 +1707,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1859,178 +1720,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2070,7 +1889,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719ED11E-0B98-3B39-BE78-8971F85E5770}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719ED11E-0B98-3B39-BE78-8971F85E5770}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2100,9 +1919,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2140,9 +1959,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2177,7 +1996,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2212,7 +2031,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2385,46 +2204,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="22.453125" customWidth="1"/>
-    <col min="9" max="9" width="32.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="32.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
-      <c r="C1" s="60" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69"/>
       <c r="H1" s="39" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
     </row>
-    <row r="2" spans="2:10">
-      <c r="H2" s="63" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
         <v>3</v>
@@ -2433,126 +2252,107 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J4" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J5" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="25"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="J6" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="14.5" customHeight="1"/>
-    <row r="8" spans="2:10">
+    <row r="7" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10">
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:10">
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:15">
-      <c r="B18" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="C20" s="35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="37"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="35"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2566,10 +2366,8 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15">
-      <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2583,218 +2381,216 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="14.5" customHeight="1">
+    <row r="24" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
-      <c r="B24" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C26" s="38"/>
     </row>
-    <row r="31" spans="1:15">
-      <c r="B31" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65"/>
-      <c r="N31" s="65"/>
-      <c r="O31" s="65"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="65"/>
-      <c r="N32" s="65"/>
-      <c r="O32" s="65"/>
-    </row>
-    <row r="33" spans="2:15">
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="65"/>
-      <c r="M33" s="65"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="65"/>
-    </row>
-    <row r="58" spans="2:15">
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="66"/>
-      <c r="F58" s="66"/>
-      <c r="G58" s="66"/>
-      <c r="H58" s="66"/>
-      <c r="I58" s="66"/>
-      <c r="J58" s="66"/>
-      <c r="K58" s="66"/>
-      <c r="L58" s="66"/>
-      <c r="M58" s="66"/>
-      <c r="N58" s="66"/>
-      <c r="O58" s="66"/>
-    </row>
-    <row r="59" spans="2:15">
-      <c r="B59" s="66" t="s">
-        <v>77</v>
-      </c>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="66"/>
-      <c r="F59" s="66"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="66"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="66"/>
-      <c r="M59" s="66"/>
-      <c r="N59" s="66"/>
-      <c r="O59" s="66"/>
-    </row>
-    <row r="60" spans="2:15">
-      <c r="B60" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="C60" s="66"/>
-      <c r="D60" s="66"/>
-      <c r="E60" s="66"/>
-      <c r="F60" s="66"/>
-      <c r="G60" s="66"/>
-      <c r="H60" s="66"/>
-      <c r="I60" s="66"/>
-      <c r="J60" s="66"/>
-      <c r="K60" s="66"/>
-      <c r="L60" s="66"/>
-      <c r="M60" s="66"/>
-      <c r="N60" s="66"/>
-      <c r="O60" s="66"/>
-    </row>
-    <row r="61" spans="2:15">
-      <c r="B61" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66"/>
-      <c r="H61" s="66"/>
-      <c r="I61" s="66"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="66"/>
-      <c r="L61" s="66"/>
-      <c r="M61" s="66"/>
-      <c r="N61" s="66"/>
-      <c r="O61" s="66"/>
-    </row>
-    <row r="62" spans="2:15">
-      <c r="B62" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" s="67"/>
-      <c r="D62" s="67"/>
-      <c r="E62" s="67"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="67"/>
-      <c r="H62" s="67"/>
-      <c r="I62" s="67"/>
-      <c r="J62" s="67"/>
-      <c r="K62" s="67"/>
-      <c r="L62" s="67"/>
-      <c r="M62" s="67"/>
-      <c r="N62" s="67"/>
-      <c r="O62" s="67"/>
-    </row>
-    <row r="63" spans="2:15">
-      <c r="B63" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="67"/>
-      <c r="D63" s="67"/>
-      <c r="E63" s="67"/>
-      <c r="F63" s="67"/>
-      <c r="G63" s="67"/>
-      <c r="H63" s="67"/>
-      <c r="I63" s="67"/>
-      <c r="J63" s="67"/>
-      <c r="K63" s="67"/>
-      <c r="L63" s="67"/>
-      <c r="M63" s="67"/>
-      <c r="N63" s="67"/>
-      <c r="O63" s="67"/>
-    </row>
-    <row r="64" spans="2:15">
-      <c r="B64" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="C64" s="67"/>
-      <c r="D64" s="67"/>
-      <c r="E64" s="67"/>
-      <c r="F64" s="67"/>
-      <c r="G64" s="67"/>
-      <c r="H64" s="67"/>
-      <c r="I64" s="67"/>
-      <c r="J64" s="67"/>
-      <c r="K64" s="67"/>
-      <c r="L64" s="67"/>
-      <c r="M64" s="67"/>
-      <c r="N64" s="67"/>
-      <c r="O64" s="67"/>
-    </row>
-    <row r="65" spans="2:15">
-      <c r="B65" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="C65" s="66"/>
-      <c r="D65" s="66"/>
-      <c r="E65" s="66"/>
-      <c r="F65" s="66"/>
-      <c r="G65" s="66"/>
-      <c r="H65" s="66"/>
-      <c r="I65" s="66"/>
-      <c r="J65" s="66"/>
-      <c r="K65" s="66"/>
-      <c r="L65" s="66"/>
-      <c r="M65" s="66"/>
-      <c r="N65" s="66"/>
-      <c r="O65" s="66"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B31" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="72"/>
+      <c r="O32" s="72"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="72"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B58" s="73"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="73"/>
+      <c r="K58" s="73"/>
+      <c r="L58" s="73"/>
+      <c r="M58" s="73"/>
+      <c r="N58" s="73"/>
+      <c r="O58" s="73"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B59" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
+      <c r="J59" s="73"/>
+      <c r="K59" s="73"/>
+      <c r="L59" s="73"/>
+      <c r="M59" s="73"/>
+      <c r="N59" s="73"/>
+      <c r="O59" s="73"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B60" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
+      <c r="F60" s="73"/>
+      <c r="G60" s="73"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="73"/>
+      <c r="M60" s="73"/>
+      <c r="N60" s="73"/>
+      <c r="O60" s="73"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B61" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="73"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="L61" s="73"/>
+      <c r="M61" s="73"/>
+      <c r="N61" s="73"/>
+      <c r="O61" s="73"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B62" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
+      <c r="G62" s="73"/>
+      <c r="H62" s="73"/>
+      <c r="I62" s="73"/>
+      <c r="J62" s="73"/>
+      <c r="K62" s="73"/>
+      <c r="L62" s="73"/>
+      <c r="M62" s="73"/>
+      <c r="N62" s="73"/>
+      <c r="O62" s="73"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B63" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
+      <c r="F63" s="73"/>
+      <c r="G63" s="73"/>
+      <c r="H63" s="73"/>
+      <c r="I63" s="73"/>
+      <c r="J63" s="73"/>
+      <c r="K63" s="73"/>
+      <c r="L63" s="73"/>
+      <c r="M63" s="73"/>
+      <c r="N63" s="73"/>
+      <c r="O63" s="73"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B64" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
+      <c r="I64" s="73"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
+      <c r="L64" s="73"/>
+      <c r="M64" s="73"/>
+      <c r="N64" s="73"/>
+      <c r="O64" s="73"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B65" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="73"/>
+      <c r="F65" s="73"/>
+      <c r="G65" s="73"/>
+      <c r="H65" s="73"/>
+      <c r="I65" s="73"/>
+      <c r="J65" s="73"/>
+      <c r="K65" s="73"/>
+      <c r="L65" s="73"/>
+      <c r="M65" s="73"/>
+      <c r="N65" s="73"/>
+      <c r="O65" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2818,150 +2614,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:Q12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" customWidth="1"/>
-    <col min="16" max="16" width="40.453125" customWidth="1"/>
+    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="16" max="16" width="40.5" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17">
-      <c r="B1" s="60" t="s">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
-    </row>
-    <row r="3" spans="2:17">
-      <c r="B3" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73"/>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="B5" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="G5" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-    </row>
-    <row r="6" spans="2:17">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="G5" s="81" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="76" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="90"/>
-    </row>
-    <row r="7" spans="2:17">
+        <v>17</v>
+      </c>
+      <c r="G6" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="94"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="68" t="s">
-        <v>84</v>
+      <c r="C7" s="74" t="s">
+        <v>111</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="77"/>
-      <c r="H7" s="89"/>
+        <v>73</v>
+      </c>
+      <c r="G7" s="83"/>
+      <c r="H7" s="93"/>
       <c r="I7" s="14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="N7" s="86" t="s">
-        <v>96</v>
-      </c>
-      <c r="O7" s="87"/>
-      <c r="P7" s="86" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q7" s="87"/>
-    </row>
-    <row r="8" spans="2:17">
+        <v>82</v>
+      </c>
+      <c r="N7" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" s="91"/>
+      <c r="P7" s="90" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="91"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E8" s="4"/>
       <c r="G8" s="46"/>
@@ -2971,55 +2767,55 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="97"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="101"/>
       <c r="P8" s="43"/>
       <c r="Q8" s="21"/>
     </row>
-    <row r="9" spans="2:17">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="68"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G9" s="14">
         <v>1</v>
       </c>
-      <c r="H9" s="2">
-        <v>2</v>
+      <c r="H9" s="65" t="s">
+        <v>113</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="J9" s="48">
         <v>45750.666666666664</v>
       </c>
       <c r="K9" s="40" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="L9" s="40" t="b">
         <v>0</v>
       </c>
       <c r="M9" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="88" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="88" t="s">
         <v>98</v>
       </c>
-      <c r="N9" s="84" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="P9" s="84" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q9" s="85"/>
-    </row>
-    <row r="10" spans="2:17">
+      <c r="Q9" s="89"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="45"/>
       <c r="D10" s="4"/>
@@ -3028,16 +2824,16 @@
         <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="J10" s="48">
         <v>45752</v>
       </c>
       <c r="K10" s="40" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="L10" s="40" t="b">
         <v>0</v>
@@ -3045,39 +2841,39 @@
       <c r="M10" s="40">
         <v>0</v>
       </c>
-      <c r="N10" s="84" t="b">
+      <c r="N10" s="88" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="96"/>
+      <c r="O10" s="100"/>
       <c r="P10" s="41" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="Q10" s="42"/>
     </row>
-    <row r="11" spans="2:17" ht="45" customHeight="1">
+    <row r="11" spans="2:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C11" s="94" t="s">
-        <v>88</v>
+      <c r="C11" s="98" t="s">
+        <v>112</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="11">
         <v>3</v>
       </c>
       <c r="H11" s="10">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J11" s="51">
+        <v>89</v>
+      </c>
+      <c r="J11" s="50">
         <v>45750.666666666664</v>
       </c>
-      <c r="K11" s="51">
+      <c r="K11" s="50">
         <v>45751.666666666664</v>
       </c>
       <c r="L11" s="12" t="b">
@@ -3086,39 +2882,39 @@
       <c r="M11" s="12">
         <v>3600</v>
       </c>
-      <c r="N11" s="80" t="b">
+      <c r="N11" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="81" t="s">
-        <v>37</v>
-      </c>
-      <c r="P11" s="80" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q11" s="81"/>
-    </row>
-    <row r="12" spans="2:17" ht="43.5">
+      <c r="O11" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q11" s="87"/>
+    </row>
+    <row r="12" spans="2:17" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
         <v>5</v>
       </c>
-      <c r="C12" s="95"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="4"/>
       <c r="E12" s="47" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="G12" s="11">
         <v>4</v>
       </c>
       <c r="H12" s="10">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="J12" s="51">
+        <v>87</v>
+      </c>
+      <c r="J12" s="50">
         <v>45748.4375</v>
       </c>
-      <c r="K12" s="51">
+      <c r="K12" s="50">
         <v>45748.375</v>
       </c>
       <c r="L12" s="12" t="b">
@@ -3127,120 +2923,120 @@
       <c r="M12" s="12">
         <v>1800</v>
       </c>
-      <c r="N12" s="80" t="b">
+      <c r="N12" s="86" t="b">
         <v>0</v>
       </c>
-      <c r="O12" s="81"/>
-      <c r="P12" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q12" s="81"/>
-    </row>
-    <row r="13" spans="2:17">
+      <c r="O12" s="87"/>
+      <c r="P12" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q12" s="87"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="4">
         <v>6</v>
       </c>
-      <c r="C13" s="69" t="s">
-        <v>35</v>
+      <c r="C13" s="75" t="s">
+        <v>25</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="14">
         <v>5</v>
       </c>
-      <c r="H13" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="83"/>
-      <c r="P13" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" s="83"/>
-    </row>
-    <row r="14" spans="2:17">
+      <c r="H13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="89"/>
+      <c r="P13" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="89"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <v>7</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="14">
         <v>6</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="L14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" s="78" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="79"/>
-      <c r="P14" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" s="83"/>
-    </row>
-    <row r="15" spans="2:17">
+      <c r="H14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="85"/>
+      <c r="P14" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" s="89"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="4">
         <v>8</v>
       </c>
-      <c r="C15" s="68" t="s">
-        <v>35</v>
+      <c r="C15" s="74" t="s">
+        <v>25</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="14">
         <v>7</v>
       </c>
-      <c r="H15" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="83"/>
-    </row>
-    <row r="16" spans="2:17">
+      <c r="H15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="89"/>
+      <c r="P15" s="88"/>
+      <c r="Q15" s="89"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="4">
         <v>9</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="11"/>
@@ -3250,17 +3046,17 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="85"/>
-      <c r="P16" s="92"/>
-      <c r="Q16" s="93"/>
-    </row>
-    <row r="17" spans="2:17">
+      <c r="N16" s="88"/>
+      <c r="O16" s="89"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="97"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <v>10</v>
       </c>
-      <c r="C17" s="68" t="s">
-        <v>35</v>
+      <c r="C17" s="74" t="s">
+        <v>25</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -3271,16 +3067,16 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="84"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="92"/>
-      <c r="Q17" s="93"/>
-    </row>
-    <row r="18" spans="2:17">
+      <c r="N17" s="88"/>
+      <c r="O17" s="89"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="97"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="4">
         <v>11</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="11"/>
@@ -3290,17 +3086,17 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="84"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="92"/>
-      <c r="Q18" s="93"/>
-    </row>
-    <row r="19" spans="2:17">
+      <c r="N18" s="88"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="97"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="4">
         <v>12</v>
       </c>
-      <c r="C19" s="68" t="s">
-        <v>35</v>
+      <c r="C19" s="74" t="s">
+        <v>25</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -3311,25 +3107,25 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="92"/>
-      <c r="Q19" s="93"/>
-    </row>
-    <row r="20" spans="2:17">
+      <c r="N19" s="88"/>
+      <c r="O19" s="89"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="97"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="4">
         <v>13</v>
       </c>
-      <c r="C20" s="68"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
+        <v>29</v>
+      </c>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -3378,154 +3174,154 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:R25"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="6" max="6" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.36328125" customWidth="1"/>
-    <col min="16" max="16" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.36328125" customWidth="1"/>
-    <col min="18" max="18" width="9.453125" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.33203125" customWidth="1"/>
+    <col min="18" max="18" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18">
-      <c r="B1" s="60" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
-    </row>
-    <row r="3" spans="2:18">
-      <c r="B3" s="102" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73"/>
-    </row>
-    <row r="5" spans="2:18">
-      <c r="B5" s="104" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B3" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="107" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-    </row>
-    <row r="6" spans="2:18" ht="14.5" customHeight="1">
+      <c r="G5" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+    </row>
+    <row r="6" spans="2:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="G6" s="76" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="88" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="105" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="105" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" s="106"/>
-    </row>
-    <row r="7" spans="2:18">
-      <c r="B7" s="69">
+      <c r="G6" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="114"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" s="109"/>
+    </row>
+    <row r="7" spans="2:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="75">
         <v>1</v>
       </c>
-      <c r="C7" s="94" t="s">
-        <v>104</v>
+      <c r="C7" s="98" t="s">
+        <v>114</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="89"/>
+        <v>92</v>
+      </c>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="M7" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" s="91"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="99"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q7" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="R7" s="87"/>
-    </row>
-    <row r="8" spans="2:18">
-      <c r="B8" s="95"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="G8" s="14">
         <v>1</v>
@@ -3533,19 +3329,17 @@
       <c r="H8" s="9">
         <v>2</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="I8" s="8"/>
       <c r="J8" s="8" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="L8" s="53">
+        <v>97</v>
+      </c>
+      <c r="L8" s="52">
         <v>45750.416666666664</v>
       </c>
-      <c r="M8" s="53">
+      <c r="M8" s="52">
         <v>45750.791666666664</v>
       </c>
       <c r="N8" s="8" t="b">
@@ -3557,35 +3351,35 @@
       <c r="P8" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" s="107" t="s">
-        <v>118</v>
-      </c>
-      <c r="R8" s="108"/>
-    </row>
-    <row r="9" spans="2:18">
-      <c r="B9" s="95"/>
-      <c r="C9" s="99"/>
+      <c r="Q8" s="110" t="s">
+        <v>100</v>
+      </c>
+      <c r="R8" s="111"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="99"/>
+      <c r="C9" s="103"/>
       <c r="D9" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="G9" s="11">
         <v>2</v>
       </c>
       <c r="H9" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="L9" s="50">
+        <v>101</v>
+      </c>
+      <c r="L9" s="49">
         <v>45750.416666666664</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="N9" s="13" t="b">
         <v>0</v>
@@ -3596,16 +3390,16 @@
       <c r="P9" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="Q9" s="109" t="s">
-        <v>99</v>
-      </c>
-      <c r="R9" s="110"/>
-    </row>
-    <row r="10" spans="2:18">
-      <c r="B10" s="95"/>
-      <c r="C10" s="99"/>
+      <c r="Q9" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="R9" s="113"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="99"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G10" s="14">
         <v>3</v>
@@ -3615,15 +3409,15 @@
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" s="53">
+        <v>87</v>
+      </c>
+      <c r="L10" s="52">
         <v>45750.416666666664</v>
       </c>
-      <c r="M10" s="53">
+      <c r="M10" s="52">
         <v>45750.417361111111</v>
       </c>
       <c r="N10" s="8" t="b">
@@ -3635,20 +3429,20 @@
       <c r="P10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="Q10" s="107" t="s">
-        <v>120</v>
-      </c>
-      <c r="R10" s="108"/>
-    </row>
-    <row r="11" spans="2:18" ht="43.5">
-      <c r="B11" s="69">
+      <c r="Q10" s="110" t="s">
+        <v>102</v>
+      </c>
+      <c r="R10" s="111"/>
+    </row>
+    <row r="11" spans="2:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="75">
         <v>2</v>
       </c>
-      <c r="C11" s="94" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>111</v>
+      <c r="C11" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>116</v>
       </c>
       <c r="G11" s="11">
         <v>4</v>
@@ -3658,15 +3452,15 @@
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" s="50">
+        <v>87</v>
+      </c>
+      <c r="L11" s="49">
         <v>45750.416666666664</v>
       </c>
-      <c r="M11" s="50">
+      <c r="M11" s="49">
         <v>45750.415972222225</v>
       </c>
       <c r="N11" s="13" t="b">
@@ -3678,70 +3472,58 @@
       <c r="P11" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="Q11" s="109" t="s">
-        <v>99</v>
-      </c>
-      <c r="R11" s="110"/>
-    </row>
-    <row r="12" spans="2:18" ht="43.5">
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="52" t="s">
-        <v>112</v>
+      <c r="Q11" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="R11" s="113"/>
+    </row>
+    <row r="12" spans="2:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="B12" s="99"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="51" t="s">
+        <v>117</v>
       </c>
       <c r="G12" s="14">
         <v>5</v>
       </c>
-      <c r="H12" s="9">
-        <v>7</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="108"/>
-    </row>
-    <row r="13" spans="2:18" ht="43.5">
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="52" t="s">
-        <v>113</v>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="111"/>
+    </row>
+    <row r="13" spans="2:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="51" t="s">
+        <v>118</v>
       </c>
       <c r="G13" s="14">
         <v>6</v>
       </c>
-      <c r="H13" s="9">
-        <v>8</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="108"/>
-    </row>
-    <row r="14" spans="2:18">
-      <c r="B14" s="69">
+      <c r="Q13" s="110"/>
+      <c r="R13" s="111"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="75">
         <v>3</v>
       </c>
-      <c r="C14" s="94"/>
+      <c r="C14" s="98"/>
       <c r="D14" s="2"/>
       <c r="G14" s="14">
         <v>7</v>
@@ -3755,12 +3537,12 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="108"/>
-    </row>
-    <row r="15" spans="2:18">
-      <c r="B15" s="95"/>
-      <c r="C15" s="99"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="111"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="99"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="2"/>
       <c r="G15" s="14">
         <v>8</v>
@@ -3774,12 +3556,12 @@
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="108"/>
-    </row>
-    <row r="16" spans="2:18">
-      <c r="B16" s="95"/>
-      <c r="C16" s="99"/>
+      <c r="Q15" s="110"/>
+      <c r="R15" s="111"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="99"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="2"/>
       <c r="G16" s="14">
         <v>9</v>
@@ -3793,12 +3575,12 @@
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="108"/>
-    </row>
-    <row r="17" spans="2:18">
-      <c r="B17" s="95"/>
-      <c r="C17" s="99"/>
+      <c r="Q16" s="110"/>
+      <c r="R16" s="111"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B17" s="99"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="2"/>
       <c r="G17" s="14">
         <v>10</v>
@@ -3812,12 +3594,12 @@
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="108"/>
-    </row>
-    <row r="18" spans="2:18">
-      <c r="B18" s="95"/>
-      <c r="C18" s="99"/>
+      <c r="Q17" s="110"/>
+      <c r="R17" s="111"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18" s="99"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="2"/>
       <c r="G18" s="14">
         <v>11</v>
@@ -3831,12 +3613,12 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="107"/>
-      <c r="R18" s="108"/>
-    </row>
-    <row r="19" spans="2:18">
-      <c r="B19" s="70"/>
-      <c r="C19" s="100"/>
+      <c r="Q18" s="110"/>
+      <c r="R18" s="111"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" s="76"/>
+      <c r="C19" s="104"/>
       <c r="D19" s="2"/>
       <c r="G19" s="14">
         <v>12</v>
@@ -3850,18 +3632,18 @@
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
       <c r="P19" s="23"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="108"/>
-    </row>
-    <row r="20" spans="2:18">
-      <c r="B20" s="69">
+      <c r="Q19" s="110"/>
+      <c r="R19" s="111"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B20" s="75">
         <v>4</v>
       </c>
-      <c r="C20" s="94" t="s">
-        <v>35</v>
+      <c r="C20" s="98" t="s">
+        <v>25</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G20" s="14">
         <v>13</v>
@@ -3875,62 +3657,60 @@
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="108"/>
-    </row>
-    <row r="21" spans="2:18">
-      <c r="B21" s="95"/>
-      <c r="C21" s="99"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="111"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" s="99"/>
+      <c r="C21" s="103"/>
       <c r="D21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18">
-      <c r="B22" s="95"/>
-      <c r="C22" s="99"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="99"/>
+      <c r="C22" s="103"/>
       <c r="D22" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18">
-      <c r="B23" s="95"/>
-      <c r="C23" s="99"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" s="99"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
-      <c r="K23" s="103"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="103"/>
+        <v>25</v>
+      </c>
+      <c r="G23" s="102"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="115"/>
+      <c r="K23" s="115"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
       <c r="N23" s="31"/>
     </row>
-    <row r="24" spans="2:18">
-      <c r="B24" s="95"/>
-      <c r="C24" s="99"/>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B24" s="99"/>
+      <c r="C24" s="103"/>
       <c r="D24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="101"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="101"/>
-      <c r="L24" s="101"/>
-      <c r="M24" s="101"/>
+        <v>25</v>
+      </c>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="105"/>
       <c r="N24" s="32"/>
     </row>
-    <row r="25" spans="2:18">
-      <c r="B25" s="70"/>
-      <c r="C25" s="100"/>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B25" s="76"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="K6:P6"/>
     <mergeCell ref="Q10:R10"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="I23:M23"/>
@@ -3948,6 +3728,8 @@
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q15:R15"/>
     <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="K6:P6"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
@@ -3972,209 +3754,209 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" customWidth="1"/>
-    <col min="13" max="13" width="30.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.1796875" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
-      <c r="B1" s="60" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
-    </row>
-    <row r="3" spans="2:14">
-      <c r="B3" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="115" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="122" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="88" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="90"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1">
-      <c r="B5" s="121"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="114"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+      <c r="N3" s="125"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="123" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="139" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="92" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="94"/>
+    </row>
+    <row r="5" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="138"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="122"/>
       <c r="F5" s="17" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="K5" s="112" t="s">
-        <v>96</v>
-      </c>
-      <c r="L5" s="113"/>
+        <v>103</v>
+      </c>
+      <c r="K5" s="118" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="119"/>
       <c r="M5" s="17" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="15" thickTop="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15">
         <v>1</v>
       </c>
-      <c r="C6" s="119" t="s">
-        <v>55</v>
+      <c r="C6" s="136" t="s">
+        <v>44</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="142" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="146" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="147">
+        <v>45</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="60">
         <v>45750.666666666664</v>
       </c>
-      <c r="H6" s="146" t="s">
+      <c r="H6" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="120" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="121" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="146" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="146" t="s">
+      <c r="N6" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="K6" s="148" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="149" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="146" t="s">
-        <v>116</v>
-      </c>
-      <c r="N6" s="157" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="7">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="119"/>
+      <c r="C7" s="136"/>
       <c r="D7" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="145" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="150">
+        <v>104</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="48">
         <v>45752</v>
       </c>
-      <c r="H7" s="145" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" s="145" t="b">
+      <c r="H7" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="145">
+      <c r="J7" s="40">
         <v>0</v>
       </c>
-      <c r="K7" s="82" t="b">
+      <c r="K7" s="88" t="b">
         <v>1</v>
       </c>
-      <c r="L7" s="83"/>
-      <c r="M7" s="54" t="s">
-        <v>117</v>
+      <c r="L7" s="89"/>
+      <c r="M7" s="41" t="s">
+        <v>99</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="7">
         <f t="shared" ref="B8" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="119"/>
+      <c r="C8" s="136"/>
       <c r="D8" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="143" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>27</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="144">
+        <v>28</v>
+      </c>
+      <c r="G8" s="58">
         <v>45750.666666666664</v>
       </c>
-      <c r="H8" s="144">
+      <c r="H8" s="58">
         <v>45751.666666666664</v>
       </c>
       <c r="I8" s="8" t="b">
@@ -4183,33 +3965,33 @@
       <c r="J8" s="8">
         <v>3600</v>
       </c>
-      <c r="K8" s="107" t="b">
+      <c r="K8" s="110" t="b">
         <v>1</v>
       </c>
-      <c r="L8" s="108"/>
+      <c r="L8" s="111"/>
       <c r="M8" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="N8" s="141" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
+        <v>86</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="7">
         <v>4</v>
       </c>
-      <c r="C9" s="119"/>
-      <c r="D9" s="55" t="s">
-        <v>123</v>
+      <c r="C9" s="136"/>
+      <c r="D9" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="144">
+        <v>87</v>
+      </c>
+      <c r="G9" s="58">
         <v>45748.4375</v>
       </c>
-      <c r="H9" s="144">
+      <c r="H9" s="58">
         <v>45748.375</v>
       </c>
       <c r="I9" s="8" t="b">
@@ -4218,36 +4000,36 @@
       <c r="J9" s="8">
         <v>1800</v>
       </c>
-      <c r="K9" s="107" t="b">
+      <c r="K9" s="110" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="108"/>
+      <c r="L9" s="111"/>
       <c r="M9" s="8" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="C10" s="119"/>
+      <c r="C10" s="136"/>
       <c r="D10" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>125</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="144">
+        <v>97</v>
+      </c>
+      <c r="G10" s="58">
         <v>45750.416666666664</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>124</v>
+      <c r="H10" s="52">
+        <v>45750.791666666664</v>
       </c>
       <c r="I10" s="8" t="b">
         <v>1</v>
@@ -4255,36 +4037,36 @@
       <c r="J10" s="8">
         <v>1800</v>
       </c>
-      <c r="K10" s="107" t="b">
+      <c r="K10" s="110" t="b">
         <v>1</v>
       </c>
-      <c r="L10" s="108"/>
+      <c r="L10" s="111"/>
       <c r="M10" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="N10" s="141" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14">
+        <v>100</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="7">
         <v>6</v>
       </c>
-      <c r="C11" s="119"/>
+      <c r="C11" s="136"/>
       <c r="D11" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>126</v>
+        <v>27</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G11" s="53">
+        <v>101</v>
+      </c>
+      <c r="G11" s="52">
         <v>45750.416666666664</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="I11" s="8" t="b">
         <v>0</v>
@@ -4292,90 +4074,90 @@
       <c r="J11" s="8">
         <v>0</v>
       </c>
-      <c r="K11" s="107" t="b">
+      <c r="K11" s="110" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="108"/>
-      <c r="M11" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="N11" s="141" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1">
-      <c r="B12" s="155">
+      <c r="L11" s="111"/>
+      <c r="M11" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="63">
         <v>7</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="58"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="151" t="s">
-        <v>100</v>
-      </c>
-      <c r="G12" s="152">
+        <v>47</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="62">
         <v>45750.416666666664</v>
       </c>
-      <c r="H12" s="152">
+      <c r="H12" s="62">
         <v>45750.416666666664</v>
       </c>
-      <c r="I12" s="151" t="b">
+      <c r="I12" s="61" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="151">
+      <c r="J12" s="61">
         <v>60</v>
       </c>
-      <c r="K12" s="153" t="b">
+      <c r="K12" s="116" t="b">
         <v>1</v>
       </c>
-      <c r="L12" s="154"/>
-      <c r="M12" s="151" t="s">
-        <v>120</v>
-      </c>
-      <c r="N12" s="156" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="15.5" thickTop="1" thickBot="1">
+      <c r="L12" s="117"/>
+      <c r="M12" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="N12" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
         <v>8</v>
       </c>
-      <c r="C13" s="120"/>
+      <c r="C13" s="137"/>
       <c r="D13" s="22" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="151" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="152">
+        <v>48</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="62">
         <v>45750.416666666664</v>
       </c>
-      <c r="H13" s="152">
+      <c r="H13" s="62">
         <v>45750.415972222225</v>
       </c>
-      <c r="I13" s="151" t="b">
+      <c r="I13" s="61" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="151">
+      <c r="J13" s="61">
         <v>60</v>
       </c>
-      <c r="K13" s="153" t="b">
+      <c r="K13" s="116" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="154"/>
-      <c r="M13" s="151" t="s">
-        <v>99</v>
-      </c>
-      <c r="N13" s="151" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1">
+      <c r="L13" s="117"/>
+      <c r="M13" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
@@ -4390,9 +4172,9 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="2:14" ht="14.5" customHeight="1">
+    <row r="15" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
@@ -4402,102 +4184,102 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
+      <c r="K15" s="148"/>
+      <c r="L15" s="148"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1">
+    <row r="16" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="2:16" ht="15" thickTop="1">
-      <c r="C17" s="130" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+    <row r="17" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="127" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="128"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="129"/>
       <c r="G17" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="130" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="133"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="132"/>
-      <c r="M17" s="130" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17" s="133"/>
-      <c r="O17" s="131"/>
-      <c r="P17" s="132"/>
-    </row>
-    <row r="18" spans="2:16" ht="14.5" customHeight="1">
-      <c r="B18" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="127" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="128" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="128" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="138" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="134" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="135"/>
-      <c r="J18" s="128" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" s="128" t="s">
-        <v>66</v>
-      </c>
-      <c r="L18" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="M18" s="139" t="s">
-        <v>70</v>
-      </c>
-      <c r="N18" s="128" t="s">
-        <v>65</v>
-      </c>
-      <c r="O18" s="128" t="s">
-        <v>66</v>
-      </c>
-      <c r="P18" s="129" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16">
-      <c r="B19" s="126"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="129"/>
-      <c r="G19" s="138"/>
-      <c r="H19" s="136"/>
-      <c r="I19" s="137"/>
-      <c r="J19" s="128"/>
-      <c r="K19" s="128"/>
-      <c r="L19" s="129"/>
-      <c r="M19" s="140"/>
-      <c r="N19" s="128"/>
-      <c r="O19" s="128"/>
-      <c r="P19" s="129"/>
-    </row>
-    <row r="20" spans="2:16">
+      <c r="H17" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="130"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="128"/>
+      <c r="L17" s="129"/>
+      <c r="M17" s="127" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="130"/>
+      <c r="O17" s="128"/>
+      <c r="P17" s="129"/>
+    </row>
+    <row r="18" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="144" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="126" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="145" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="131" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="132"/>
+      <c r="J18" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="L18" s="145" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" s="146" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="P18" s="145" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B19" s="143"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="126"/>
+      <c r="K19" s="126"/>
+      <c r="L19" s="145"/>
+      <c r="M19" s="147"/>
+      <c r="N19" s="126"/>
+      <c r="O19" s="126"/>
+      <c r="P19" s="145"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="30" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C20" s="26">
         <v>8</v>
@@ -4508,14 +4290,14 @@
       <c r="E20" s="28">
         <v>0</v>
       </c>
-      <c r="F20" s="158" t="s">
-        <v>127</v>
+      <c r="F20" s="64" t="s">
+        <v>108</v>
       </c>
       <c r="G20" s="34"/>
-      <c r="H20" s="124" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="125"/>
+      <c r="H20" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="142"/>
       <c r="J20" s="2">
         <v>0</v>
       </c>
@@ -4526,7 +4308,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="N20" s="2">
         <v>0</v>
@@ -4538,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M21" s="3"/>
     </row>
   </sheetData>
@@ -4551,8 +4333,6 @@
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="N18:N19"/>
     <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B18:B19"/>
@@ -4580,6 +4360,8 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4588,6 +4370,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -4731,7 +4519,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4740,13 +4528,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EFF49E-866D-4BFD-B7FD-9BB436667B53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4764,19 +4555,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>